<commit_message>
Add Shield/Shield_absorption.xlsx + update
</commit_message>
<xml_diff>
--- a/Design_Guide/Copper_thickness.xlsx
+++ b/Design_Guide/Copper_thickness.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylvain Rouland\Desktop\Design_Guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylvain Rouland\Desktop\PCB\Design_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53A3E7F-2402-4971-A772-5BAF7B49CEB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE514C61-1B8C-46D7-A6EB-4B590EA191B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF0EFF3B-76B3-47ED-B534-93142EAE8B03}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{CF0EFF3B-76B3-47ED-B534-93142EAE8B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -433,13 +436,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA90295-5BED-4572-8A01-FDEA0EB8BF1A}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" style="1" customWidth="1"/>
@@ -447,7 +450,7 @@
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -530,7 +533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -547,7 +550,7 @@
         <v>17.143643837849474</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -564,7 +567,7 @@
         <v>34.287287675698948</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -581,7 +584,7 @@
         <v>68.574575351397897</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -598,7 +601,7 @@
         <v>102.86186302709685</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -615,7 +618,7 @@
         <v>137.14915070279579</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -632,7 +635,7 @@
         <v>171.43643837849473</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -649,7 +652,7 @@
         <v>205.72372605419369</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -666,7 +669,7 @@
         <v>240.01101372989262</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>8</v>
       </c>
@@ -683,7 +686,7 @@
         <v>274.29830140559159</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -700,7 +703,7 @@
         <v>308.58558908129055</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -715,6 +718,57 @@
       <c r="D22" s="1">
         <f t="shared" si="2"/>
         <v>342.87287675698946</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" ref="B23:B25" si="3">A23*$B$1</f>
+        <v>311.85000000000002</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" ref="C23:C25" si="4">B23/$B$4</f>
+        <v>35.039325842696627</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" ref="D23:D25" si="5">10000*C23/$B$3</f>
+        <v>377.16016443268836</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="3"/>
+        <v>340.20000000000005</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="4"/>
+        <v>38.224719101123597</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="5"/>
+        <v>411.44745210838738</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="3"/>
+        <v>368.55</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="4"/>
+        <v>41.41011235955056</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="5"/>
+        <v>445.73473978408629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>